<commit_message>
power capacity data update
</commit_message>
<xml_diff>
--- a/data/Power Capacity.xlsx
+++ b/data/Power Capacity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Documents\Rpackages\china_co2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4CE9AD-C266-47E1-BB25-63B4E161562F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF47291-6BA8-45A5-BE00-ABDD6C00CC4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1577" yWindow="-103" windowWidth="31440" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="2200" windowWidth="27540" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Newly-added Installed Capacity " sheetId="1" r:id="rId1"/>
@@ -176,27 +176,6 @@
     <t>Time Period</t>
   </si>
   <si>
-    <t>2008-12:2023-04</t>
-  </si>
-  <si>
-    <t>2010-09:2023-04</t>
-  </si>
-  <si>
-    <t>2009-12:2023-04</t>
-  </si>
-  <si>
-    <t>2017-12:2023-04</t>
-  </si>
-  <si>
-    <t>2012-12:2023-04</t>
-  </si>
-  <si>
-    <t>2020-06:2023-04</t>
-  </si>
-  <si>
-    <t>2018-02:2023-04</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -209,13 +188,34 @@
     <t>Update</t>
   </si>
   <si>
-    <t>2023-05-22</t>
+    <t>2008-12:2023-05</t>
   </si>
   <si>
-    <t>2023-05-25</t>
+    <t>2010-09:2023-05</t>
   </si>
   <si>
-    <t>2023-05-24</t>
+    <t>2009-12:2023-05</t>
+  </si>
+  <si>
+    <t>2017-12:2023-05</t>
+  </si>
+  <si>
+    <t>2012-12:2023-05</t>
+  </si>
+  <si>
+    <t>2020-06:2023-05</t>
+  </si>
+  <si>
+    <t>2018-02:2023-05</t>
+  </si>
+  <si>
+    <t>2023-06-21</t>
+  </si>
+  <si>
+    <t>2023-06-30</t>
+  </si>
+  <si>
+    <t>2023-06-29</t>
   </si>
 </sst>
 </file>
@@ -616,9 +616,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q164"/>
+  <dimension ref="A1:Q165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -855,110 +855,110 @@
         <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="P7" s="4" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>50</v>
@@ -9275,6 +9275,59 @@
       </c>
       <c r="Q164" s="3">
         <v>44050</v>
+      </c>
+    </row>
+    <row r="165" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A165" s="2">
+        <v>45077</v>
+      </c>
+      <c r="B165" s="3">
+        <v>434</v>
+      </c>
+      <c r="C165" s="3">
+        <v>2202</v>
+      </c>
+      <c r="D165" s="3">
+        <v>119</v>
+      </c>
+      <c r="E165" s="3">
+        <v>1636</v>
+      </c>
+      <c r="F165" s="3">
+        <v>6121</v>
+      </c>
+      <c r="G165" s="3">
+        <v>1522</v>
+      </c>
+      <c r="H165" s="3">
+        <v>340</v>
+      </c>
+      <c r="I165" s="3">
+        <v>267240</v>
+      </c>
+      <c r="J165" s="3">
+        <v>41700</v>
+      </c>
+      <c r="K165" s="3">
+        <v>135095</v>
+      </c>
+      <c r="L165" s="3">
+        <v>5676</v>
+      </c>
+      <c r="M165" s="3">
+        <v>38260</v>
+      </c>
+      <c r="N165" s="3">
+        <v>36881</v>
+      </c>
+      <c r="O165" s="3">
+        <v>113679</v>
+      </c>
+      <c r="P165" s="3">
+        <v>11871</v>
+      </c>
+      <c r="Q165" s="3">
+        <v>45392</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to data and workflows for 2023Q2
</commit_message>
<xml_diff>
--- a/data/Power Capacity.xlsx
+++ b/data/Power Capacity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauri\Documents\Rpackages\china_co2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB6971F-E5FF-42CF-9120-64F2EC66758A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53D5DE2-5810-4089-924B-CC47DE18EEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="2200" windowWidth="27540" windowHeight="15860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1570" yWindow="-110" windowWidth="36940" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Newly-added Installed Capacity " sheetId="1" r:id="rId1"/>
@@ -188,19 +188,7 @@
     <t>Update</t>
   </si>
   <si>
-    <t>2008-12:2023-05</t>
-  </si>
-  <si>
-    <t>2010-09:2023-05</t>
-  </si>
-  <si>
-    <t>2009-12:2023-05</t>
-  </si>
-  <si>
     <t>2017-12:2023-05</t>
-  </si>
-  <si>
-    <t>2012-12:2023-05</t>
   </si>
   <si>
     <t>2020-06:2023-05</t>
@@ -209,13 +197,25 @@
     <t>2018-02:2023-05</t>
   </si>
   <si>
-    <t>2023-06-21</t>
-  </si>
-  <si>
     <t>2023-06-30</t>
   </si>
   <si>
     <t>2023-06-29</t>
+  </si>
+  <si>
+    <t>2008-12:2023-06</t>
+  </si>
+  <si>
+    <t>2010-09:2023-06</t>
+  </si>
+  <si>
+    <t>2009-12:2023-06</t>
+  </si>
+  <si>
+    <t>2012-12:2023-06</t>
+  </si>
+  <si>
+    <t>2023-07-21</t>
   </si>
 </sst>
 </file>
@@ -616,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q165"/>
+  <dimension ref="A1:Q166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -855,52 +855,52 @@
         <v>38</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="I6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="P6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q6" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.35">
@@ -961,52 +961,52 @@
         <v>42</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="P8" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.35">
@@ -9328,6 +9328,59 @@
       </c>
       <c r="Q165" s="3">
         <v>45392</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A166" s="2">
+        <v>45107</v>
+      </c>
+      <c r="B166" s="3">
+        <v>536</v>
+      </c>
+      <c r="C166" s="3">
+        <v>2602</v>
+      </c>
+      <c r="D166" s="3">
+        <v>119</v>
+      </c>
+      <c r="E166" s="3">
+        <v>2299</v>
+      </c>
+      <c r="F166" s="3">
+        <v>7842</v>
+      </c>
+      <c r="G166" s="3">
+        <v>0</v>
+      </c>
+      <c r="H166" s="3">
+        <v>0</v>
+      </c>
+      <c r="I166" s="3">
+        <v>270772</v>
+      </c>
+      <c r="J166" s="3">
+        <v>41793</v>
+      </c>
+      <c r="K166" s="3">
+        <v>135698</v>
+      </c>
+      <c r="L166" s="3">
+        <v>5676</v>
+      </c>
+      <c r="M166" s="3">
+        <v>38921</v>
+      </c>
+      <c r="N166" s="3">
+        <v>0</v>
+      </c>
+      <c r="O166" s="3">
+        <v>0</v>
+      </c>
+      <c r="P166" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q166" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>